<commit_message>
fix titel stiercode v5
</commit_message>
<xml_diff>
--- a/Stierenkaart/Prijslijst.xlsx
+++ b/Stierenkaart/Prijslijst.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kisamen.sharepoint.com/sites/financieleadministratie/Gedeelde documenten/General/_Kris/Indexdraai/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kisamen-my.sharepoint.com/personal/v_vanrooijen_kisamen_com/Documents/Bureaublad/Project Stierenkaart/Stierenkaart/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{1E3992E1-0A1D-493D-9FC3-9B9112505B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -14030,9 +14030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB54933E-7B8D-404B-B44C-9C980107D408}">
   <dimension ref="A1:D2384"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -40510,15 +40508,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="fccaa644-1360-4841-a670-28c1fa4382ee">
@@ -40529,14 +40518,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7D7DDAC-CECB-4729-AF74-7FF405219112}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7D7DDAC-CECB-4729-AF74-7FF405219112}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fccaa644-1360-4841-a670-28c1fa4382ee"/>
+    <ds:schemaRef ds:uri="0f38339f-8a74-43ff-91a2-6ab9ac7e5793"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94CDB1FF-5ECF-4406-884E-A406B935AE59}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{858C3F07-3BEB-47F4-AF4D-D884719DD273}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fccaa644-1360-4841-a670-28c1fa4382ee"/>
+    <ds:schemaRef ds:uri="0f38339f-8a74-43ff-91a2-6ab9ac7e5793"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{858C3F07-3BEB-47F4-AF4D-D884719DD273}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94CDB1FF-5ECF-4406-884E-A406B935AE59}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>